<commit_message>
recomender system, rt removed before ts
</commit_message>
<xml_diff>
--- a/app/static/csv/for_participant.xlsx
+++ b/app/static/csv/for_participant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FB46FE-5F27-4AF3-82D6-98235A9CA040}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C98F2A2-9181-45AD-A35D-34626A6FF155}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="for_participant" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="262">
   <si>
     <t>tag</t>
   </si>
@@ -790,6 +791,24 @@
   </si>
   <si>
     <t>Arko Ghosh, Afdeling Cognitieve Psychologie, Instituut Psychologie, Universiteit Leiden agestudy@fsw.leidenuniv.nl</t>
+  </si>
+  <si>
+    <t>p24a</t>
+  </si>
+  <si>
+    <t>You may also be compensated for referring the data collection platform to a friend at the rate of 5 EUR per a successful referral. This compensation is only available if you reside in the Netherlands (as is any compensation in this study). A referral is considered successful only if the referred user uses the unique promotion code passed-on by you during the registration, and remains in the study for a period of 1 year. After this period, the reward amount can be requested for payment together with your bank details as explained above. You will be able to review the number of referrals on your dashboard at any time (when logged-in). This referral rewards program will become unavailable for new referrals as soon as the target recruitment is completed and you shall be explicitly informed of this via this website dashboard (when logged-in). This is entirely optional and has no other bearing on the study.</t>
+  </si>
+  <si>
+    <t>p24b</t>
+  </si>
+  <si>
+    <t>For University of Leiden students performing online tasks, the following reward structure applies. 1 Credit is offered for 30 min of online tasks. This corresponds to performing 2 recommended online tasks for 1 Credit, and a maximum of 4 credits can be obtained by performing 8 recommended tasks. The minimum duration for remaining in the study to receive any credit is 2 months. It is possible to remain in the study for paid or voluntary participation upon termination of the credit period and then general participation commitment applies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U kunt ook een beloning van 5 euro verdienen door iemand succesvol naar de het onderzoek te verwijzen. Deze beloning is alleen beschikbaar als u in Nederland woont (dat geldt voor elke betaling voor deze studie). Een verwijzing geldt alleen als succesvol als de persoon die verwezen is tijdens de registratie de unieke promotiecode invoert die u hebt gegeven, en een jaar lang deel blijft nemen aan het onderzoek. Na deze periode kan de beloning worden opgevraagd onder vermelding van de bankgegevens, zoals hierboven is uitgelegd. U kunt het aantal verwijzingen altijd inzien op uw dashboard (als u ingelogd bent). Zodra het beoogde aantal deelnemers bereikt is zal de mogelijkheid om geld te krijgen voor verwijzingen worden beëindigd. Hierover word u expliciet geïnformeerd via uw dashboard (als u ingelogd bent). Het staat u vrij om wel of niet mee te doen met het verwijzen van deelnemers. Dit heeft verder geen gevolgen voor de studie. </t>
+  </si>
+  <si>
+    <t>Voor studenten van de Universiteit Leiden die aan online taken deelnemen gelden de volgende beloningsregels. Er wordt 1 SONA credit toegekend voor 30 minuten online-testdeelname. Dit komt overeen met het doorlopen van twee aanbevolen online tests voor 1 credit. Er kunnen maximaal 4 credits worden behaald door 8 aanbevolen taken uit te voeren. U moet minimaal twee maanden aan de studie blijven deelnemen om credits te kunnen verdienen. Na de minimum periode die voor credit beloning geldt is het mogelijk om betaald of vrijwillig door te gaan met de studie. Vanaf dat moment gelden de algemene deelnameregels.</t>
   </si>
 </sst>
 </file>
@@ -1663,10 +1682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1845,7 +1864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="232" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2186,7 +2205,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -2340,278 +2359,300 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>131</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>132</v>
+        <v>256</v>
+      </c>
+      <c r="B62" t="s">
+        <v>257</v>
       </c>
       <c r="C62" t="s">
-        <v>133</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>258</v>
       </c>
       <c r="B63" t="s">
-        <v>162</v>
+        <v>259</v>
       </c>
       <c r="C63" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>136</v>
-      </c>
-      <c r="B64" t="s">
-        <v>161</v>
+        <v>131</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="C64" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B66" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B67" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C67" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B68" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C68" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B69" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C69" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B70" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C70" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B71" t="s">
-        <v>253</v>
+        <v>156</v>
       </c>
       <c r="C71" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B72" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C72" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="B73" t="s">
-        <v>189</v>
+        <v>253</v>
       </c>
       <c r="C73" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="B74" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="C74" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
+        <v>189</v>
       </c>
       <c r="C75" t="s">
-        <v>238</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B76" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C76" t="s">
-        <v>239</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B77" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C77" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>180</v>
       </c>
       <c r="C78" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B79" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C79" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B80" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C80" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B81" t="s">
-        <v>179</v>
+        <v>245</v>
       </c>
       <c r="C81" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B82" t="s">
-        <v>175</v>
+        <v>244</v>
       </c>
       <c r="C82" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B83" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C83" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B84" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C84" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B85" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C85" t="s">
-        <v>255</v>
+        <v>182</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>184</v>
+      </c>
+      <c r="B86" t="s">
+        <v>186</v>
+      </c>
+      <c r="C86" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>185</v>
+      </c>
+      <c r="B87" t="s">
+        <v>187</v>
+      </c>
+      <c r="C87" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>190</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B88" t="s">
         <v>191</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C88" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2622,6 +2663,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2630,7 +2677,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D896C3867AA3F4EB0C0DE718E7AD517" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80024e68534539ed8e026f0b5c1f9e6f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c478e2cf-1bd2-4bab-9bac-f508c15c8b21" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dc892a718835b0a8dea2591f8ec0eaf" ns3:_="">
     <xsd:import namespace="c478e2cf-1bd2-4bab-9bac-f508c15c8b21"/>
@@ -2808,13 +2855,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A153F602-4523-4BE8-B1FF-29BC7BE3DF9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CBCEA50-9F8E-445F-8351-E21F5791CC1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2822,7 +2872,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{571203FD-96FA-4C52-A5CD-CF8F121E2059}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2838,13 +2888,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A153F602-4523-4BE8-B1FF-29BC7BE3DF9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
remove ability to collect payment
</commit_message>
<xml_diff>
--- a/app/static/csv/for_participant.xlsx
+++ b/app/static/csv/for_participant.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="337">
   <si>
     <t>tag</t>
   </si>
@@ -46,10 +46,10 @@
     <t>li2</t>
   </si>
   <si>
-    <t>Step 2. Install the &lt;a href=/about_app&gt;App&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Stap 2. Installeer de &lt;a href=/about_app&gt;App&lt;/a&gt;</t>
+    <t>Step 2. Install the app via the &lt;a href=/about_app&gt;Google Play Store&lt;/a&gt; or  &lt;a href=/about_app_apple&gt;Apple App Store&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Stap 2. Installeer de app via  &lt;a href=/about_app&gt;Google Play Store&lt;/a&gt; of &lt;a href=/about_app_apple&gt;Apple App Store&lt;/a&gt;</t>
   </si>
   <si>
     <t>li3</t>
@@ -691,7 +691,7 @@
     <t>li_data_2</t>
   </si>
   <si>
-    <t xml:space="preserve">The University of Leiden and IBM cloud or similar. All the email correspondences and email addresses stored in agestudy@fsw.leidenuniv.nl will be deleted at the end of the study period. </t>
+    <t xml:space="preserve">Psytoolkit.org, Strasbourg (Online tests). The coded online testing data will be temporarily stored on the research server administered by Psytoolkit.org (Strasbourg) and stored within the UK/EU until it is downloaded in Leiden. The server is managed by Prof. Sijsbert Stoet. The data on the Psytoolkit server will be disconnected from any demographic information or email. After data collection is completed the data will be deleted from this server and according to Psytoolkit, the deletion will take 24 hours to impact their servers as well. Therefore, the long-term data will be stored at Leiden and released from Leiden. </t>
   </si>
   <si>
     <t xml:space="preserve">Psytoolkit.org, Straatsburg (Online tests). De gecodeerde gegevens van online tests worden tijdelijk opgeslagen op de onderzoeksserver beheerd door Psytoolkit.org (Straatsburg) en opgeslagen binnen het VK/EU totdat ze in Leiden worden gedownload. De server wordt beheerd door prof. Sijsbert Stoet. De gegevens op de Psytoolkit-server worden losgekoppeld van alle demografische informatie of e-mail. Na voltooiing van de gegevensverzameling worden de gegevens van deze server verwijderd en volgens Psytoolkit duurt het 24 uur voordat deze verwijdering van invloed is op hun servers. Daarom worden de langetermijngegevens opgeslagen in Leiden en vanuit Leiden vrijgegeven.     </t>
@@ -700,10 +700,10 @@
     <t>li_data_3</t>
   </si>
   <si>
-    <t>Leiden University and IBM cloud. The email address for signing up on the online tests is stored on the IBM cloud in the EU. All the email correspondence and email addresses stored in agestudy@fsw.leidenuniv.nl will be deleted at the end of the study period. Moreover, at the end of the study period the email address stored in the IBM cloud will also be deleted . All your data and the corresponding analysis will be reported to the public in anonymized form. When deposited anonymously in a public platform your data may be further processed by the scientific community to discover new patterns of behavior or new brain-behavior relationships and age effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Universiteit Leiden en IBM-cloud of vergelijkbaar. Alle e-mailcorrespondentie en e-mailadressen opgeslagen in agestudy@fsw.leidenuniv.nl worden verwijderd aan het einde van de onderzoeksperiode. Bovendien wordt het e-mailadres opgeslagen in de cloud (gelegen in de EU en losgekoppeld van de database die wordt gebruikt voor het verwerken van smartphonegegevens via Quantactions) tijdens de aanmelding op het online testplatform ook verwijderd aan het einde van de onderzoeksperiode.  </t>
+    <t>Leiden University and Microsoft Azure. The email address for signing up on the online tests is stored on  Microsoft Azure cloud services in the EU. All the email correspondence and email addresses stored in agestudy@fsw.leidenuniv.nl will be deleted at the end of the study period. Moreover, at the end of the study period the email address stored in Azure will also be deleted . All your data and the corresponding analysis will be reported to the public in anonymized form. When deposited anonymously in a public platform your data may be further processed by the scientific community to discover new patterns of behavior or new brain-behavior relationships and age effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Universiteit Leiden enMicrosoft  Azure of vergelijkbaar. Alle e-mailcorrespondentie en e-mailadressen opgeslagen in agestudy@fsw.leidenuniv.nl worden verwijderd aan het einde van de onderzoeksperiode. Bovendien wordt het e-mailadres opgeslagen in de Microsoft Azure cloud (gelegen in de EU en losgekoppeld van de database die wordt gebruikt voor het verwerken van smartphonegegevens via Quantactions) tijdens de aanmelding op het online testplatform ook verwijderd aan het einde van de onderzoeksperiode.  </t>
   </si>
   <si>
     <t>p19b</t>
@@ -727,10 +727,10 @@
     <t>h24</t>
   </si>
   <si>
-    <t>Compensation</t>
-  </si>
-  <si>
-    <t>Vergoeding</t>
+    <t>Compensation (Unfortunately we are unable to accept participation for compensation at this time)</t>
+  </si>
+  <si>
+    <t>Vergoeding (Helaas kunnen wij op dit moment geen deelname tegen vergoeding meer accepteren)</t>
   </si>
   <si>
     <t>p21_u</t>
@@ -965,6 +965,15 @@
   </si>
   <si>
     <t xml:space="preserve">Voor meer informatie over gegevensprivacy en uw rechten, raadpleegt u alstublieft de wetgeving inzake gegevensbescherming van de Europese Unie, bekend als de Algemene Verordening Gegevensbescherming (“AVG”). </t>
+  </si>
+  <si>
+    <t>p27c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: Your withdrawal from the study can only be executed once you install the App from your phone. If you wish to continue using the App after withdrawal, uninstall and reinstall again.  </t>
+  </si>
+  <si>
+    <t>LET OP: Je uitschrijving uit de studie kan alleen worden uitgevoerd nadat je de app op je telefoon hebt geïnstalleerd. Als je na uitschrijving wilt doorgaan met het gebruik van de app, deïnstalleer deze dan en installeer hem opnieuw.</t>
   </si>
   <si>
     <t>h27</t>
@@ -1047,7 +1056,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1065,12 +1074,6 @@
       <sz val="10"/>
       <color rgb="FF3d3c40"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1120,8 +1123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -1134,20 +1140,20 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1454,25 +1460,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="255.57642857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="255.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="255.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="255.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1480,10 +1486,10 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1491,10 +1497,10 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1502,10 +1508,10 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1513,10 +1519,10 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1524,10 +1530,10 @@
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1535,10 +1541,10 @@
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1546,10 +1552,10 @@
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1557,10 +1563,10 @@
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1568,10 +1574,10 @@
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1579,32 +1585,32 @@
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="4">
-      <c r="A12" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="4">
-      <c r="A13" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1612,10 +1618,10 @@
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1623,10 +1629,10 @@
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1634,11 +1640,11 @@
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="57" customFormat="1" s="4">
-      <c r="A17" s="5" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="57" customFormat="1" s="5">
+      <c r="A17" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1652,10 +1658,10 @@
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1663,10 +1669,10 @@
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1674,10 +1680,10 @@
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1685,10 +1691,10 @@
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1696,10 +1702,10 @@
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1707,10 +1713,10 @@
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1718,10 +1724,10 @@
       <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1729,10 +1735,10 @@
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1740,18 +1746,18 @@
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A27" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A27" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -1762,18 +1768,18 @@
       <c r="A28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A29" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A29" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="6" t="s">
         <v>82</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -1784,18 +1790,18 @@
       <c r="A30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A31" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A31" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -1806,29 +1812,29 @@
       <c r="A32" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A33" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A33" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="6" t="s">
         <v>94</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A34" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A34" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -1839,18 +1845,18 @@
       <c r="A35" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A36" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A36" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>103</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -1861,18 +1867,18 @@
       <c r="A37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A38" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A38" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="6" t="s">
         <v>109</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -1883,10 +1889,10 @@
       <c r="A39" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1894,10 +1900,10 @@
       <c r="A40" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1905,10 +1911,10 @@
       <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1916,10 +1922,10 @@
       <c r="A42" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1927,10 +1933,10 @@
       <c r="A43" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1938,10 +1944,10 @@
       <c r="A44" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1949,10 +1955,10 @@
       <c r="A45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1960,10 +1966,10 @@
       <c r="A46" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1971,10 +1977,10 @@
       <c r="A47" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="2" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1982,10 +1988,10 @@
       <c r="A48" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1993,10 +1999,10 @@
       <c r="A49" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2004,10 +2010,10 @@
       <c r="A50" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2015,10 +2021,10 @@
       <c r="A51" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2026,10 +2032,10 @@
       <c r="A52" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2037,10 +2043,10 @@
       <c r="A53" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2048,10 +2054,10 @@
       <c r="A54" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2059,10 +2065,10 @@
       <c r="A55" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="2" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2070,10 +2076,10 @@
       <c r="A56" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2081,10 +2087,10 @@
       <c r="A57" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2092,10 +2098,10 @@
       <c r="A58" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2103,10 +2109,10 @@
       <c r="A59" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2114,10 +2120,10 @@
       <c r="A60" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2125,10 +2131,10 @@
       <c r="A61" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="2" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2136,10 +2142,10 @@
       <c r="A62" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2147,10 +2153,10 @@
       <c r="A63" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2158,10 +2164,10 @@
       <c r="A64" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2169,10 +2175,10 @@
       <c r="A65" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2180,10 +2186,10 @@
       <c r="A66" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="2" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2191,10 +2197,10 @@
       <c r="A67" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="2" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2202,10 +2208,10 @@
       <c r="A68" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="2" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2213,21 +2219,21 @@
       <c r="A69" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A70" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A70" s="6" t="s">
         <v>202</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="6" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2235,10 +2241,10 @@
       <c r="A71" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="2" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2246,10 +2252,10 @@
       <c r="A72" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2257,10 +2263,10 @@
       <c r="A73" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="2" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2268,18 +2274,18 @@
       <c r="A74" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A75" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A75" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="6" t="s">
         <v>218</v>
       </c>
       <c r="C75" s="7" t="s">
@@ -2290,10 +2296,10 @@
       <c r="A76" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="2" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2301,10 +2307,10 @@
       <c r="A77" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="2" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2312,10 +2318,10 @@
       <c r="A78" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="2" t="s">
         <v>228</v>
       </c>
     </row>
@@ -2323,10 +2329,10 @@
       <c r="A79" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="2" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2337,7 +2343,7 @@
       <c r="B80" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="2" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2345,10 +2351,10 @@
       <c r="A81" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="2" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2356,10 +2362,10 @@
       <c r="A82" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="2" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2367,10 +2373,10 @@
       <c r="A83" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="2" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2378,10 +2384,10 @@
       <c r="A84" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="2" t="s">
         <v>246</v>
       </c>
     </row>
@@ -2389,10 +2395,10 @@
       <c r="A85" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="2" t="s">
         <v>249</v>
       </c>
     </row>
@@ -2400,21 +2406,21 @@
       <c r="A86" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="21.75">
       <c r="A87" s="1" t="s">
         <v>253</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="2" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2422,10 +2428,10 @@
       <c r="A88" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="2" t="s">
         <v>258</v>
       </c>
     </row>
@@ -2433,10 +2439,10 @@
       <c r="A89" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="2" t="s">
         <v>261</v>
       </c>
     </row>
@@ -2444,10 +2450,10 @@
       <c r="A90" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="2" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2455,10 +2461,10 @@
       <c r="A91" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="2" t="s">
         <v>267</v>
       </c>
     </row>
@@ -2466,10 +2472,10 @@
       <c r="A92" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="2" t="s">
         <v>270</v>
       </c>
     </row>
@@ -2477,10 +2483,10 @@
       <c r="A93" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -2488,10 +2494,10 @@
       <c r="A94" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="2" t="s">
         <v>276</v>
       </c>
     </row>
@@ -2499,10 +2505,10 @@
       <c r="A95" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="2" t="s">
         <v>279</v>
       </c>
     </row>
@@ -2510,10 +2516,10 @@
       <c r="A96" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="2" t="s">
         <v>282</v>
       </c>
     </row>
@@ -2521,10 +2527,10 @@
       <c r="A97" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="2" t="s">
         <v>285</v>
       </c>
     </row>
@@ -2532,10 +2538,10 @@
       <c r="A98" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="2" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2543,10 +2549,10 @@
       <c r="A99" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="2" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2554,10 +2560,10 @@
       <c r="A100" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="2" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2565,10 +2571,10 @@
       <c r="A101" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="2" t="s">
         <v>297</v>
       </c>
     </row>
@@ -2576,10 +2582,10 @@
       <c r="A102" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="2" t="s">
         <v>300</v>
       </c>
     </row>
@@ -2587,10 +2593,10 @@
       <c r="A103" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="2" t="s">
         <v>303</v>
       </c>
     </row>
@@ -2598,10 +2604,10 @@
       <c r="A104" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="2" t="s">
         <v>306</v>
       </c>
     </row>
@@ -2609,10 +2615,10 @@
       <c r="A105" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="2" t="s">
         <v>309</v>
       </c>
     </row>
@@ -2620,10 +2626,10 @@
       <c r="A106" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="2" t="s">
         <v>312</v>
       </c>
     </row>
@@ -2631,10 +2637,10 @@
       <c r="A107" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="2" t="s">
         <v>315</v>
       </c>
     </row>
@@ -2642,10 +2648,10 @@
       <c r="A108" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="2" t="s">
         <v>318</v>
       </c>
     </row>
@@ -2653,10 +2659,10 @@
       <c r="A109" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="2" t="s">
         <v>321</v>
       </c>
     </row>
@@ -2664,10 +2670,10 @@
       <c r="A110" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="2" t="s">
         <v>324</v>
       </c>
     </row>
@@ -2675,10 +2681,10 @@
       <c r="A111" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="2" t="s">
         <v>327</v>
       </c>
     </row>
@@ -2686,10 +2692,10 @@
       <c r="A112" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B112" s="9" t="s">
+      <c r="B112" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="2" t="s">
         <v>330</v>
       </c>
     </row>
@@ -2697,11 +2703,22 @@
       <c r="A113" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="2" t="s">
         <v>333</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
+      <c r="A114" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>